<commit_message>
added condition to check if email present
</commit_message>
<xml_diff>
--- a/MemberData.xlsx
+++ b/MemberData.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/siyadms/Documents/workspace/AMIA/mailSender/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/siyadms/Documents/workspace/AMIA/meetingOrganser/mailSender/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="860" yWindow="460" windowWidth="24740" windowHeight="15540" tabRatio="500"/>
+    <workbookView xWindow="900" yWindow="460" windowWidth="24700" windowHeight="15540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>ID</t>
   </si>
@@ -57,12 +57,6 @@
   </si>
   <si>
     <t>siyadms@gmail.com</t>
-  </si>
-  <si>
-    <t>Naseeha</t>
-  </si>
-  <si>
-    <t>naseehas1988@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -424,7 +418,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="A3" sqref="A3:H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -492,30 +486,14 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="1">
-        <v>434549</v>
-      </c>
-      <c r="G3" s="1">
-        <v>1</v>
-      </c>
-      <c r="H3" s="1">
-        <v>3</v>
-      </c>
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
@@ -560,7 +538,6 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1"/>
-    <hyperlink ref="E3" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>